<commit_message>
Corporate APNs DB GUI
</commit_message>
<xml_diff>
--- a/Test excel.xlsx
+++ b/Test excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>MTX Name</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>ggsnlab</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Corporate APNs</t>
   </si>
 </sst>
 </file>
@@ -395,27 +401,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -424,7 +438,7 @@
         <v>05</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -433,7 +447,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -442,7 +456,7 @@
         <v>07</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -451,7 +465,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -460,7 +474,7 @@
         <v>09</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -469,7 +483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -478,7 +492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -487,7 +501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -496,7 +510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -505,7 +519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>

</xml_diff>